<commit_message>
[update] seperate flation from procedure so to add dtype check
</commit_message>
<xml_diff>
--- a/assets/autofin/autofin_mock_20241101.xlsx
+++ b/assets/autofin/autofin_mock_20241101.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22185" windowHeight="9135" activeTab="1"/>
+    <workbookView windowWidth="22185" windowHeight="9135" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="autofin_pretrial" sheetId="1" r:id="rId1"/>
@@ -1528,7 +1528,7 @@
     <t>org_addr</t>
   </si>
   <si>
-    <t>orgname</t>
+    <t>org_name</t>
   </si>
   <si>
     <t>rep_certno</t>
@@ -5522,8 +5522,8 @@
   <sheetPr/>
   <dimension ref="A1:AT15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -12656,8 +12656,8 @@
   <sheetPr/>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25:G26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5" outlineLevelCol="7"/>

</xml_diff>